<commit_message>
sql test file added
</commit_message>
<xml_diff>
--- a/output/spreadsheets/indirect_costs.xlsx
+++ b/output/spreadsheets/indirect_costs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,818 +520,1274 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Apr-15</t>
+          <t>Mar-15</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>266766.05</v>
+        <v>160742.94</v>
       </c>
       <c r="D5" t="n">
-        <v>64937.04</v>
+        <v>38995.74</v>
       </c>
       <c r="E5" t="n">
-        <v>331703.09</v>
+        <v>199738.68</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>May-15</t>
+          <t>Apr-15</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>262059.38</v>
+        <v>256056.24</v>
       </c>
       <c r="D6" t="n">
-        <v>65636.77</v>
+        <v>64213.55</v>
       </c>
       <c r="E6" t="n">
-        <v>327696.15</v>
+        <v>320269.79</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Jun-15</t>
+          <t>Apr-15</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>260316.98</v>
+        <v>168995.27</v>
       </c>
       <c r="D7" t="n">
-        <v>62965.63</v>
+        <v>39896.76</v>
       </c>
       <c r="E7" t="n">
-        <v>323282.61</v>
+        <v>208892.03</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Jul-15</t>
+          <t>May-15</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>263297.01</v>
+        <v>260284.16</v>
       </c>
       <c r="D8" t="n">
-        <v>57104.35</v>
+        <v>57556.92</v>
       </c>
       <c r="E8" t="n">
-        <v>320401.36</v>
+        <v>317841.08</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Aug-15</t>
+          <t>May-15</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" t="n">
-        <v>254281.27</v>
+        <v>167195.28</v>
       </c>
       <c r="D9" t="n">
-        <v>58385.58</v>
+        <v>40195.44</v>
       </c>
       <c r="E9" t="n">
-        <v>312666.85</v>
+        <v>207390.72</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Sep-15</t>
+          <t>Jun-15</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>252867.21</v>
+        <v>256414.89</v>
       </c>
       <c r="D10" t="n">
-        <v>61618.76</v>
+        <v>61346.3</v>
       </c>
       <c r="E10" t="n">
-        <v>314485.97</v>
+        <v>317761.19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Oct-15</t>
+          <t>Jun-15</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" t="n">
-        <v>317542.44</v>
+        <v>170945.33</v>
       </c>
       <c r="D11" t="n">
-        <v>72687.45</v>
+        <v>37761.88</v>
       </c>
       <c r="E11" t="n">
-        <v>390229.89</v>
+        <v>208707.21</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Nov-15</t>
+          <t>Jul-15</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>262180.98</v>
+        <v>267660.8</v>
       </c>
       <c r="D12" t="n">
-        <v>59029.8</v>
+        <v>61584.04</v>
       </c>
       <c r="E12" t="n">
-        <v>321210.78</v>
+        <v>329244.84</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Dec-15</t>
+          <t>Jul-15</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" t="n">
-        <v>258650.74</v>
+        <v>178058.27</v>
       </c>
       <c r="D13" t="n">
-        <v>55717.72</v>
+        <v>36528.44</v>
       </c>
       <c r="E13" t="n">
-        <v>314368.46</v>
+        <v>214586.71</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Jan-16</t>
+          <t>Aug-15</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>252175.98</v>
+        <v>262457.27</v>
       </c>
       <c r="D14" t="n">
-        <v>58329.03</v>
+        <v>62696.12</v>
       </c>
       <c r="E14" t="n">
-        <v>310505.01</v>
+        <v>325153.39</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Feb-16</t>
+          <t>Aug-15</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" t="n">
-        <v>244305.23</v>
+        <v>175032.39</v>
       </c>
       <c r="D15" t="n">
-        <v>60012.48</v>
+        <v>41534.43</v>
       </c>
       <c r="E15" t="n">
-        <v>304317.71</v>
+        <v>216566.82</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Mar-16</t>
+          <t>Sep-15</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>241621.2</v>
+        <v>258928.32</v>
       </c>
       <c r="D16" t="n">
-        <v>58528.24</v>
+        <v>61834.99</v>
       </c>
       <c r="E16" t="n">
-        <v>300149.44</v>
+        <v>320763.31</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Apr-16</t>
+          <t>Sep-15</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" t="n">
-        <v>239032.88</v>
+        <v>175960.43</v>
       </c>
       <c r="D17" t="n">
-        <v>63694.36</v>
+        <v>48544.6</v>
       </c>
       <c r="E17" t="n">
-        <v>302727.24</v>
+        <v>224505.03</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>May-16</t>
+          <t>Oct-15</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>1</v>
       </c>
       <c r="C18" t="n">
-        <v>239635.18</v>
+        <v>259209.61</v>
       </c>
       <c r="D18" t="n">
-        <v>57655.44</v>
+        <v>58787.85</v>
       </c>
       <c r="E18" t="n">
-        <v>297290.62</v>
+        <v>317997.46</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Jun-16</t>
+          <t>Oct-15</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19" t="n">
-        <v>243293.68</v>
+        <v>183109.08</v>
       </c>
       <c r="D19" t="n">
-        <v>54036.96</v>
+        <v>42289.25</v>
       </c>
       <c r="E19" t="n">
-        <v>297330.64</v>
+        <v>225398.33</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Jul-16</t>
+          <t>Nov-15</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>1</v>
       </c>
       <c r="C20" t="n">
-        <v>242000.98</v>
+        <v>259236.71</v>
       </c>
       <c r="D20" t="n">
-        <v>50080.31</v>
+        <v>54222.69</v>
       </c>
       <c r="E20" t="n">
-        <v>292081.29</v>
+        <v>313459.4</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Aug-16</t>
+          <t>Nov-15</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21" t="n">
-        <v>234265.6</v>
+        <v>174740.62</v>
       </c>
       <c r="D21" t="n">
-        <v>54302.69</v>
+        <v>43348.3</v>
       </c>
       <c r="E21" t="n">
-        <v>288568.29</v>
+        <v>218088.92</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Sep-16</t>
+          <t>Dec-15</t>
         </is>
       </c>
       <c r="B22" t="n">
         <v>1</v>
       </c>
       <c r="C22" t="n">
-        <v>240823.88</v>
+        <v>260436.51</v>
       </c>
       <c r="D22" t="n">
-        <v>56481.26</v>
+        <v>58130.84</v>
       </c>
       <c r="E22" t="n">
-        <v>297305.14</v>
+        <v>318567.35</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Oct-16</t>
+          <t>Dec-15</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23" t="n">
-        <v>240985.37</v>
+        <v>175739.22</v>
       </c>
       <c r="D23" t="n">
-        <v>56440.75</v>
+        <v>42108.26</v>
       </c>
       <c r="E23" t="n">
-        <v>297426.12</v>
+        <v>217847.48</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Nov-16</t>
+          <t>Jan-16</t>
         </is>
       </c>
       <c r="B24" t="n">
         <v>1</v>
       </c>
       <c r="C24" t="n">
-        <v>235683.88</v>
+        <v>248265.01</v>
       </c>
       <c r="D24" t="n">
-        <v>55490.59</v>
+        <v>57011.33</v>
       </c>
       <c r="E24" t="n">
-        <v>291174.47</v>
+        <v>305276.34</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Dec-16</t>
+          <t>Jan-16</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" t="n">
-        <v>239454</v>
+        <v>173373.97</v>
       </c>
       <c r="D25" t="n">
-        <v>60608.13</v>
+        <v>45299.31</v>
       </c>
       <c r="E25" t="n">
-        <v>300062.13</v>
+        <v>218673.28</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Jan-17</t>
+          <t>Feb-16</t>
         </is>
       </c>
       <c r="B26" t="n">
         <v>1</v>
       </c>
       <c r="C26" t="n">
-        <v>246937.87</v>
+        <v>249659.04</v>
       </c>
       <c r="D26" t="n">
-        <v>55133.21</v>
+        <v>53004.35</v>
       </c>
       <c r="E26" t="n">
-        <v>302071.08</v>
+        <v>302663.39</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Feb-17</t>
+          <t>Feb-16</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C27" t="n">
-        <v>252190.31</v>
+        <v>174967.91</v>
       </c>
       <c r="D27" t="n">
-        <v>56895.6</v>
+        <v>42312.91</v>
       </c>
       <c r="E27" t="n">
-        <v>309085.91</v>
+        <v>217280.82</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Mar-17</t>
+          <t>Mar-16</t>
         </is>
       </c>
       <c r="B28" t="n">
         <v>1</v>
       </c>
       <c r="C28" t="n">
-        <v>251274.75</v>
+        <v>243872.28</v>
       </c>
       <c r="D28" t="n">
-        <v>61204.42</v>
+        <v>57653.59</v>
       </c>
       <c r="E28" t="n">
-        <v>312479.17</v>
+        <v>301525.87</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Mar-17</t>
+          <t>Mar-16</t>
         </is>
       </c>
       <c r="B29" t="n">
         <v>2</v>
       </c>
       <c r="C29" t="n">
-        <v>157838.05</v>
+        <v>178150</v>
       </c>
       <c r="D29" t="n">
-        <v>39476.69</v>
+        <v>44434.03</v>
       </c>
       <c r="E29" t="n">
-        <v>197314.74</v>
+        <v>222584.03</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Apr-17</t>
+          <t>Apr-16</t>
         </is>
       </c>
       <c r="B30" t="n">
         <v>1</v>
       </c>
       <c r="C30" t="n">
-        <v>251198.9</v>
+        <v>238906.38</v>
       </c>
       <c r="D30" t="n">
-        <v>60819.21</v>
+        <v>56976.27</v>
       </c>
       <c r="E30" t="n">
-        <v>312018.11</v>
+        <v>295882.65</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Apr-17</t>
+          <t>Apr-16</t>
         </is>
       </c>
       <c r="B31" t="n">
         <v>2</v>
       </c>
       <c r="C31" t="n">
-        <v>171568.08</v>
+        <v>175385.34</v>
       </c>
       <c r="D31" t="n">
-        <v>44592.65</v>
+        <v>45371.2</v>
       </c>
       <c r="E31" t="n">
-        <v>216160.73</v>
+        <v>220756.54</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>May-17</t>
+          <t>May-16</t>
         </is>
       </c>
       <c r="B32" t="n">
         <v>1</v>
       </c>
       <c r="C32" t="n">
-        <v>253987.06</v>
+        <v>237134.48</v>
       </c>
       <c r="D32" t="n">
-        <v>61241.44</v>
+        <v>56748.89</v>
       </c>
       <c r="E32" t="n">
-        <v>315228.5</v>
+        <v>293883.37</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>May-17</t>
+          <t>May-16</t>
         </is>
       </c>
       <c r="B33" t="n">
         <v>2</v>
       </c>
       <c r="C33" t="n">
-        <v>171633.89</v>
+        <v>166381.91</v>
       </c>
       <c r="D33" t="n">
-        <v>40541.37</v>
+        <v>39407.9</v>
       </c>
       <c r="E33" t="n">
-        <v>212175.26</v>
+        <v>205789.81</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Jun-17</t>
+          <t>Jun-16</t>
         </is>
       </c>
       <c r="B34" t="n">
         <v>1</v>
       </c>
       <c r="C34" t="n">
-        <v>262773.7</v>
+        <v>241764.6</v>
       </c>
       <c r="D34" t="n">
-        <v>66451.07000000001</v>
+        <v>60886.09</v>
       </c>
       <c r="E34" t="n">
-        <v>329224.77</v>
+        <v>302650.69</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Jun-17</t>
+          <t>Jun-16</t>
         </is>
       </c>
       <c r="B35" t="n">
         <v>2</v>
       </c>
       <c r="C35" t="n">
-        <v>177504.44</v>
+        <v>166379.95</v>
       </c>
       <c r="D35" t="n">
-        <v>45522.27</v>
+        <v>42616.75</v>
       </c>
       <c r="E35" t="n">
-        <v>223026.71</v>
+        <v>208996.7</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Jul-17</t>
+          <t>Jul-16</t>
         </is>
       </c>
       <c r="B36" t="n">
         <v>1</v>
       </c>
       <c r="C36" t="n">
-        <v>265056.75</v>
+        <v>241689.72</v>
       </c>
       <c r="D36" t="n">
-        <v>62818.52</v>
+        <v>57185.97</v>
       </c>
       <c r="E36" t="n">
-        <v>327875.27</v>
+        <v>298875.69</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Jul-17</t>
+          <t>Jul-16</t>
         </is>
       </c>
       <c r="B37" t="n">
         <v>2</v>
       </c>
       <c r="C37" t="n">
-        <v>182889.46</v>
+        <v>168269.36</v>
       </c>
       <c r="D37" t="n">
-        <v>49743.53</v>
+        <v>45698.84</v>
       </c>
       <c r="E37" t="n">
-        <v>232632.99</v>
+        <v>213968.2</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Aug-17</t>
+          <t>Aug-16</t>
         </is>
       </c>
       <c r="B38" t="n">
         <v>1</v>
       </c>
       <c r="C38" t="n">
-        <v>263873.91</v>
+        <v>239990.58</v>
       </c>
       <c r="D38" t="n">
-        <v>67897.89</v>
+        <v>61696.1</v>
       </c>
       <c r="E38" t="n">
-        <v>331771.8</v>
+        <v>301686.68</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Aug-17</t>
+          <t>Aug-16</t>
         </is>
       </c>
       <c r="B39" t="n">
         <v>2</v>
       </c>
       <c r="C39" t="n">
-        <v>169786.71</v>
+        <v>155189.91</v>
       </c>
       <c r="D39" t="n">
-        <v>49554.15</v>
+        <v>45241.16</v>
       </c>
       <c r="E39" t="n">
-        <v>219340.86</v>
+        <v>200431.07</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Sep-17</t>
+          <t>Sep-16</t>
         </is>
       </c>
       <c r="B40" t="n">
         <v>1</v>
       </c>
       <c r="C40" t="n">
-        <v>263355.37</v>
+        <v>240313.86</v>
       </c>
       <c r="D40" t="n">
-        <v>64444.52</v>
+        <v>58766.4</v>
       </c>
       <c r="E40" t="n">
-        <v>327799.89</v>
+        <v>299080.26</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Sep-17</t>
+          <t>Sep-16</t>
         </is>
       </c>
       <c r="B41" t="n">
         <v>2</v>
       </c>
       <c r="C41" t="n">
-        <v>177047.06</v>
+        <v>161965.42</v>
       </c>
       <c r="D41" t="n">
-        <v>40558.19</v>
+        <v>37059.63</v>
       </c>
       <c r="E41" t="n">
-        <v>217605.25</v>
+        <v>199025.05</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Oct-17</t>
+          <t>Oct-16</t>
         </is>
       </c>
       <c r="B42" t="n">
         <v>1</v>
       </c>
       <c r="C42" t="n">
-        <v>260527.51</v>
+        <v>240012.32</v>
       </c>
       <c r="D42" t="n">
-        <v>64528.36</v>
+        <v>59436.24</v>
       </c>
       <c r="E42" t="n">
-        <v>325055.87</v>
+        <v>299448.56</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Oct-17</t>
+          <t>Oct-16</t>
         </is>
       </c>
       <c r="B43" t="n">
         <v>2</v>
       </c>
       <c r="C43" t="n">
-        <v>187165.17</v>
+        <v>172751.37</v>
       </c>
       <c r="D43" t="n">
-        <v>40507.13</v>
+        <v>37343.68</v>
       </c>
       <c r="E43" t="n">
-        <v>227672.3</v>
+        <v>210095.05</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Nov-17</t>
+          <t>Nov-16</t>
         </is>
       </c>
       <c r="B44" t="n">
         <v>1</v>
       </c>
       <c r="C44" t="n">
-        <v>254801.87</v>
+        <v>238319.46</v>
       </c>
       <c r="D44" t="n">
-        <v>61604.87</v>
+        <v>57591.61</v>
       </c>
       <c r="E44" t="n">
-        <v>316406.74</v>
+        <v>295911.07</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Nov-17</t>
+          <t>Nov-16</t>
         </is>
       </c>
       <c r="B45" t="n">
         <v>2</v>
       </c>
       <c r="C45" t="n">
-        <v>188351.17</v>
+        <v>176416.56</v>
       </c>
       <c r="D45" t="n">
-        <v>42882.99</v>
+        <v>40172.23</v>
       </c>
       <c r="E45" t="n">
-        <v>231234.16</v>
+        <v>216588.79</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Dec-17</t>
+          <t>Dec-16</t>
         </is>
       </c>
       <c r="B46" t="n">
         <v>1</v>
       </c>
       <c r="C46" t="n">
-        <v>251893.34</v>
+        <v>240254.26</v>
       </c>
       <c r="D46" t="n">
-        <v>62884.28</v>
+        <v>60005.85</v>
       </c>
       <c r="E46" t="n">
-        <v>314777.62</v>
+        <v>300260.11</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
+          <t>Dec-16</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>2</v>
+      </c>
+      <c r="C47" t="n">
+        <v>175283.73</v>
+      </c>
+      <c r="D47" t="n">
+        <v>43737.57</v>
+      </c>
+      <c r="E47" t="n">
+        <v>219021.3</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Jan-17</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>1</v>
+      </c>
+      <c r="C48" t="n">
+        <v>241911.7</v>
+      </c>
+      <c r="D48" t="n">
+        <v>59090.7</v>
+      </c>
+      <c r="E48" t="n">
+        <v>301002.4</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Jan-17</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>2</v>
+      </c>
+      <c r="C49" t="n">
+        <v>173387.7</v>
+      </c>
+      <c r="D49" t="n">
+        <v>38527.77</v>
+      </c>
+      <c r="E49" t="n">
+        <v>211915.47</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Feb-17</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>1</v>
+      </c>
+      <c r="C50" t="n">
+        <v>249348.41</v>
+      </c>
+      <c r="D50" t="n">
+        <v>60792.92</v>
+      </c>
+      <c r="E50" t="n">
+        <v>310141.33</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Feb-17</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>2</v>
+      </c>
+      <c r="C51" t="n">
+        <v>175544.71</v>
+      </c>
+      <c r="D51" t="n">
+        <v>39869.01</v>
+      </c>
+      <c r="E51" t="n">
+        <v>215413.72</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Mar-17</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>1</v>
+      </c>
+      <c r="C52" t="n">
+        <v>245877</v>
+      </c>
+      <c r="D52" t="n">
+        <v>59932.55</v>
+      </c>
+      <c r="E52" t="n">
+        <v>305809.55</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Mar-17</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>2</v>
+      </c>
+      <c r="C53" t="n">
+        <v>175935.54</v>
+      </c>
+      <c r="D53" t="n">
+        <v>39048.2</v>
+      </c>
+      <c r="E53" t="n">
+        <v>214983.74</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Apr-17</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>1</v>
+      </c>
+      <c r="C54" t="n">
+        <v>251825.11</v>
+      </c>
+      <c r="D54" t="n">
+        <v>62354.46</v>
+      </c>
+      <c r="E54" t="n">
+        <v>314179.57</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Apr-17</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>2</v>
+      </c>
+      <c r="C55" t="n">
+        <v>188537.22</v>
+      </c>
+      <c r="D55" t="n">
+        <v>41859.57</v>
+      </c>
+      <c r="E55" t="n">
+        <v>230396.79</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>May-17</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C56" t="n">
+        <v>257984.21</v>
+      </c>
+      <c r="D56" t="n">
+        <v>62318.97</v>
+      </c>
+      <c r="E56" t="n">
+        <v>320303.18</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>May-17</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>2</v>
+      </c>
+      <c r="C57" t="n">
+        <v>175769.02</v>
+      </c>
+      <c r="D57" t="n">
+        <v>42809.13</v>
+      </c>
+      <c r="E57" t="n">
+        <v>218578.15</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Jun-17</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C58" t="n">
+        <v>260625.04</v>
+      </c>
+      <c r="D58" t="n">
+        <v>70422.25</v>
+      </c>
+      <c r="E58" t="n">
+        <v>331047.29</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Jun-17</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>2</v>
+      </c>
+      <c r="C59" t="n">
+        <v>178798.33</v>
+      </c>
+      <c r="D59" t="n">
+        <v>44414.19</v>
+      </c>
+      <c r="E59" t="n">
+        <v>223212.52</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Jul-17</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>1</v>
+      </c>
+      <c r="C60" t="n">
+        <v>261607.26</v>
+      </c>
+      <c r="D60" t="n">
+        <v>63084.26</v>
+      </c>
+      <c r="E60" t="n">
+        <v>324691.52</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Jul-17</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>2</v>
+      </c>
+      <c r="C61" t="n">
+        <v>187432.86</v>
+      </c>
+      <c r="D61" t="n">
+        <v>46663.82</v>
+      </c>
+      <c r="E61" t="n">
+        <v>234096.68</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Aug-17</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>1</v>
+      </c>
+      <c r="C62" t="n">
+        <v>266230.15</v>
+      </c>
+      <c r="D62" t="n">
+        <v>60189.49</v>
+      </c>
+      <c r="E62" t="n">
+        <v>326419.64</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Aug-17</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>2</v>
+      </c>
+      <c r="C63" t="n">
+        <v>192965.39</v>
+      </c>
+      <c r="D63" t="n">
+        <v>40978.34</v>
+      </c>
+      <c r="E63" t="n">
+        <v>233943.73</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Sep-17</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>1</v>
+      </c>
+      <c r="C64" t="n">
+        <v>266774.3</v>
+      </c>
+      <c r="D64" t="n">
+        <v>68294.14999999999</v>
+      </c>
+      <c r="E64" t="n">
+        <v>335068.45</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Sep-17</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>2</v>
+      </c>
+      <c r="C65" t="n">
+        <v>182734.07</v>
+      </c>
+      <c r="D65" t="n">
+        <v>40657.16</v>
+      </c>
+      <c r="E65" t="n">
+        <v>223391.23</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Oct-17</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>1</v>
+      </c>
+      <c r="C66" t="n">
+        <v>263510.02</v>
+      </c>
+      <c r="D66" t="n">
+        <v>63688.93</v>
+      </c>
+      <c r="E66" t="n">
+        <v>327198.95</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Oct-17</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>2</v>
+      </c>
+      <c r="C67" t="n">
+        <v>174064.5</v>
+      </c>
+      <c r="D67" t="n">
+        <v>42315.52</v>
+      </c>
+      <c r="E67" t="n">
+        <v>216380.02</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Nov-17</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>1</v>
+      </c>
+      <c r="C68" t="n">
+        <v>254558.82</v>
+      </c>
+      <c r="D68" t="n">
+        <v>64080.31</v>
+      </c>
+      <c r="E68" t="n">
+        <v>318639.13</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Nov-17</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>2</v>
+      </c>
+      <c r="C69" t="n">
+        <v>172093.88</v>
+      </c>
+      <c r="D69" t="n">
+        <v>47469.49</v>
+      </c>
+      <c r="E69" t="n">
+        <v>219563.37</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
           <t>Dec-17</t>
         </is>
       </c>
-      <c r="B47" t="n">
-        <v>2</v>
-      </c>
-      <c r="C47" t="n">
-        <v>183690.09</v>
-      </c>
-      <c r="D47" t="n">
-        <v>45750.52</v>
-      </c>
-      <c r="E47" t="n">
-        <v>229440.61</v>
+      <c r="B70" t="n">
+        <v>1</v>
+      </c>
+      <c r="C70" t="n">
+        <v>250056.43</v>
+      </c>
+      <c r="D70" t="n">
+        <v>61480.02</v>
+      </c>
+      <c r="E70" t="n">
+        <v>311536.45</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Dec-17</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>2</v>
+      </c>
+      <c r="C71" t="n">
+        <v>178887.94</v>
+      </c>
+      <c r="D71" t="n">
+        <v>41287.35</v>
+      </c>
+      <c r="E71" t="n">
+        <v>220175.29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>